<commit_message>
New versions of work plan & architecture
</commit_message>
<xml_diff>
--- a/proposal/gfx/project-plan.xlsx
+++ b/proposal/gfx/project-plan.xlsx
@@ -970,7 +970,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:AF1048576"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1783,7 +1783,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Final changes for proposal submission incl. spell check
</commit_message>
<xml_diff>
--- a/proposal/gfx/project-plan.xlsx
+++ b/proposal/gfx/project-plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="460" windowWidth="37000" windowHeight="21140"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="37340" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplaner" sheetId="1" r:id="rId1"/>
@@ -483,80 +483,80 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="11" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="2" xfId="3" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="12" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="11" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="2" xfId="3" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -970,7 +970,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -996,173 +996,173 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="2:32" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>7</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="20" t="s">
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="17"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
     </row>
     <row r="3" spans="2:32" s="4" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="28"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
     </row>
     <row r="4" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26">
         <v>1</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="26">
         <v>2</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="26">
         <v>3</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="26">
         <v>4</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="26">
         <v>5</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="26">
         <v>6</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="26">
         <v>7</v>
       </c>
-      <c r="O4" s="32">
+      <c r="O4" s="26">
         <v>8</v>
       </c>
-      <c r="P4" s="32">
+      <c r="P4" s="26">
         <v>9</v>
       </c>
-      <c r="Q4" s="32">
+      <c r="Q4" s="26">
         <v>10</v>
       </c>
-      <c r="R4" s="32">
+      <c r="R4" s="26">
         <v>11</v>
       </c>
-      <c r="S4" s="32">
+      <c r="S4" s="26">
         <v>12</v>
       </c>
-      <c r="T4" s="32">
+      <c r="T4" s="26">
         <v>13</v>
       </c>
-      <c r="U4" s="32">
+      <c r="U4" s="26">
         <v>14</v>
       </c>
-      <c r="V4" s="32">
+      <c r="V4" s="26">
         <v>15</v>
       </c>
-      <c r="W4" s="32">
+      <c r="W4" s="26">
         <v>16</v>
       </c>
-      <c r="X4" s="32">
+      <c r="X4" s="26">
         <v>17</v>
       </c>
-      <c r="Y4" s="32">
+      <c r="Y4" s="26">
         <v>18</v>
       </c>
-      <c r="Z4" s="32">
+      <c r="Z4" s="26">
         <v>19</v>
       </c>
-      <c r="AA4" s="32">
+      <c r="AA4" s="26">
         <v>20</v>
       </c>
-      <c r="AB4" s="32">
+      <c r="AB4" s="26">
         <v>21</v>
       </c>
-      <c r="AC4" s="32">
+      <c r="AC4" s="26">
         <v>22</v>
       </c>
-      <c r="AD4" s="32">
+      <c r="AD4" s="26">
         <v>23</v>
       </c>
-      <c r="AE4" s="32">
+      <c r="AE4" s="26">
         <v>24</v>
       </c>
-      <c r="AF4" s="32">
+      <c r="AF4" s="26">
         <v>25</v>
       </c>
     </row>
@@ -1170,522 +1170,522 @@
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>4</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>1</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>4</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="33"/>
-      <c r="AC5" s="33"/>
-      <c r="AD5" s="33"/>
-      <c r="AE5" s="33"/>
-      <c r="AF5" s="33"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="27"/>
+      <c r="AF5" s="27"/>
     </row>
     <row r="6" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>4</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>4</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>4</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>4</v>
       </c>
       <c r="G6" s="6">
         <v>0.75</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="33"/>
-      <c r="AC6" s="33"/>
-      <c r="AD6" s="33"/>
-      <c r="AE6" s="33"/>
-      <c r="AF6" s="33"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="27"/>
+      <c r="AE6" s="27"/>
+      <c r="AF6" s="27"/>
     </row>
     <row r="7" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>7</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>2</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="6">
         <v>0.25</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="33"/>
-      <c r="AC7" s="33"/>
-      <c r="AD7" s="33"/>
-      <c r="AE7" s="33"/>
-      <c r="AF7" s="33"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>8</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>2</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="6">
         <v>0</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="33"/>
-      <c r="AC8" s="33"/>
-      <c r="AD8" s="33"/>
-      <c r="AE8" s="33"/>
-      <c r="AF8" s="33"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="27"/>
+      <c r="AF8" s="27"/>
     </row>
     <row r="9" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>10</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>7</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="6">
         <v>0</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="33"/>
-      <c r="AC9" s="33"/>
-      <c r="AD9" s="33"/>
-      <c r="AE9" s="33"/>
-      <c r="AF9" s="33"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="27"/>
+      <c r="AF9" s="27"/>
     </row>
     <row r="10" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>17</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>1</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="6">
         <v>0</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="33"/>
-      <c r="AC10" s="33"/>
-      <c r="AD10" s="33"/>
-      <c r="AE10" s="33"/>
-      <c r="AF10" s="33"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="27"/>
+      <c r="AC10" s="27"/>
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="27"/>
+      <c r="AF10" s="27"/>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>18</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>1</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="6">
         <v>0</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="33"/>
-      <c r="AD11" s="33"/>
-      <c r="AE11" s="33"/>
-      <c r="AF11" s="33"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="27"/>
+      <c r="AD11" s="27"/>
+      <c r="AE11" s="27"/>
+      <c r="AF11" s="27"/>
     </row>
     <row r="12" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>19</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>2</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="6">
         <v>0</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="33"/>
-      <c r="AC12" s="33"/>
-      <c r="AD12" s="33"/>
-      <c r="AE12" s="33"/>
-      <c r="AF12" s="33"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="27"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="27"/>
+      <c r="AF12" s="27"/>
     </row>
     <row r="13" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>21</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>4</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="6">
         <v>0</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="33"/>
-      <c r="AC13" s="33"/>
-      <c r="AD13" s="33"/>
-      <c r="AE13" s="33"/>
-      <c r="AF13" s="33"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="27"/>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>25</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>1</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="6">
         <v>0</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="33"/>
-      <c r="AC14" s="33"/>
-      <c r="AD14" s="33"/>
-      <c r="AE14" s="33"/>
-      <c r="AF14" s="33"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="27"/>
     </row>
     <row r="15" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="29">
         <v>43017</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="33"/>
-      <c r="AC15" s="33"/>
-      <c r="AD15" s="33"/>
-      <c r="AE15" s="33"/>
-      <c r="AF15" s="33"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="27"/>
+      <c r="AC15" s="27"/>
+      <c r="AD15" s="27"/>
+      <c r="AE15" s="27"/>
+      <c r="AF15" s="27"/>
     </row>
     <row r="16" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="36">
-        <v>42823</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="33"/>
-      <c r="AC16" s="33"/>
-      <c r="AD16" s="33"/>
-      <c r="AE16" s="33"/>
-      <c r="AF16" s="33"/>
+      <c r="C16" s="30">
+        <v>43188</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="27"/>
+      <c r="AC16" s="27"/>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="27"/>
+      <c r="AF16" s="27"/>
     </row>
     <row r="17" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="33"/>
-      <c r="AC17" s="33"/>
-      <c r="AD17" s="33"/>
-      <c r="AE17" s="33"/>
-      <c r="AF17" s="33"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="27"/>
+      <c r="AC17" s="27"/>
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="27"/>
+      <c r="AF17" s="27"/>
     </row>
     <row r="18" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8"/>

</xml_diff>